<commit_message>
updating the esp32 code
</commit_message>
<xml_diff>
--- a/reading form serial for ed values.xlsx
+++ b/reading form serial for ed values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\chair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{652B4D1F-E0FF-43E1-997C-FDED1ED1EB5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3552F7-03CB-4558-87CC-5598709A9F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{F1275A62-3172-4A82-84EB-A307A7F86091}"/>
+    <workbookView xWindow="14196" yWindow="996" windowWidth="17280" windowHeight="8964" xr2:uid="{F1275A62-3172-4A82-84EB-A307A7F86091}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+  <si>
+    <t>1-256</t>
+  </si>
+  <si>
+    <t>0-255</t>
+  </si>
+  <si>
+    <t>input form serial</t>
+  </si>
+  <si>
+    <t>the value in the esp</t>
+  </si>
+  <si>
+    <t>257-512</t>
+  </si>
+  <si>
+    <t>513-768</t>
+  </si>
+  <si>
+    <t>769-1024</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -381,65 +409,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C78514C-5581-49CD-9407-9C4FD8848AC5}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A4:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K2" sqref="A1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>256</v>
-      </c>
-      <c r="D1">
-        <f>(B1+1)</f>
-        <v>257</v>
-      </c>
-      <c r="E1">
-        <f>(D1+256)</f>
-        <v>513</v>
-      </c>
-      <c r="G1">
-        <f>E1+1</f>
-        <v>514</v>
-      </c>
-      <c r="H1">
-        <f>G1+256</f>
-        <v>770</v>
-      </c>
-      <c r="J1">
-        <f>H1+1</f>
-        <v>771</v>
-      </c>
-      <c r="K1">
-        <f>J1+256</f>
-        <v>1027</v>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <f>B1-A1</f>
-        <v>256</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="B2:K2" si="0">E1-D1</f>
-        <v>256</v>
-      </c>
-      <c r="G2">
-        <f t="shared" ref="G2" si="1">H1-G1</f>
-        <v>256</v>
-      </c>
-      <c r="J2">
-        <f>K1-J1</f>
-        <v>256</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>